<commit_message>
postpatient creation and token creation
</commit_message>
<xml_diff>
--- a/src/test/resources/Team01_APINinja_Data.xlsx
+++ b/src/test/resources/Team01_APINinja_Data.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shanj\vino-workspace\Team01_API_Ninja\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C3E64B9-E20A-430C-9544-7AC72CD2B734}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A56662E9-A8DB-4C20-859F-CCC0E4472ED8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="732" yWindow="732" windowWidth="17280" windowHeight="8964" xr2:uid="{A03F8C01-D493-49E0-BA62-9B2727C7C8D7}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{A03F8C01-D493-49E0-BA62-9B2727C7C8D7}"/>
   </bookViews>
   <sheets>
     <sheet name="AdminLogin" sheetId="1" r:id="rId1"/>
+    <sheet name="PatientPost" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>password</t>
   </si>
@@ -48,13 +49,58 @@
   </si>
   <si>
     <t>Team1.admin@gmail.com</t>
+  </si>
+  <si>
+    <t>FirstName</t>
+  </si>
+  <si>
+    <t>LastName</t>
+  </si>
+  <si>
+    <t>PatientContactNumber</t>
+  </si>
+  <si>
+    <t>PatientEmail</t>
+  </si>
+  <si>
+    <t>Allergy</t>
+  </si>
+  <si>
+    <t>FoodPreference</t>
+  </si>
+  <si>
+    <t>CuisineCategory</t>
+  </si>
+  <si>
+    <t>PatientDateOfBirth</t>
+  </si>
+  <si>
+    <t>Kay</t>
+  </si>
+  <si>
+    <t>KAy123@gmail.com</t>
+  </si>
+  <si>
+    <t>SOY</t>
+  </si>
+  <si>
+    <t>Vegan</t>
+  </si>
+  <si>
+    <t>Indian</t>
+  </si>
+  <si>
+    <t>Raja</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -69,6 +115,12 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -92,9 +144,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -432,7 +488,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62A42F3D-E348-4D43-8D41-01127598F126}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
@@ -463,4 +519,84 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2761C07-8EEF-424C-8E2D-5544ABDA6E0C}">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.21875" style="2" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="4">
+        <v>3248649876</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="3">
+        <v>44177</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{25FC5110-ABF1-4FD8-A244-EDF356B3C1F3}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Commit for Dietitian POST phase1
</commit_message>
<xml_diff>
--- a/src/test/resources/Team01_APINinja_Data.xlsx
+++ b/src/test/resources/Team01_APINinja_Data.xlsx
@@ -2,41 +2,31 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shanj\vino-workspace\Team01_API_Ninja\src\test\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Team 1_RestAssured_Shreya\Team01_APINinja_RestAssured\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C3E64B9-E20A-430C-9544-7AC72CD2B734}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{671F2152-892C-40F2-8C65-867E25E10276}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="732" yWindow="732" windowWidth="17280" windowHeight="8964" xr2:uid="{A03F8C01-D493-49E0-BA62-9B2727C7C8D7}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{A03F8C01-D493-49E0-BA62-9B2727C7C8D7}"/>
   </bookViews>
   <sheets>
     <sheet name="AdminLogin" sheetId="1" r:id="rId1"/>
+    <sheet name="DietitianPost" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>password</t>
   </si>
@@ -48,6 +38,60 @@
   </si>
   <si>
     <t>Team1.admin@gmail.com</t>
+  </si>
+  <si>
+    <t>ContactNumber</t>
+  </si>
+  <si>
+    <t>Education</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Firstname</t>
+  </si>
+  <si>
+    <t>HospitalCity</t>
+  </si>
+  <si>
+    <t>HospitalName</t>
+  </si>
+  <si>
+    <t>HospitalPincode</t>
+  </si>
+  <si>
+    <t>HospitalStreet</t>
+  </si>
+  <si>
+    <t>Lastname</t>
+  </si>
+  <si>
+    <t>Mphars</t>
+  </si>
+  <si>
+    <t>Hartford</t>
+  </si>
+  <si>
+    <t>Saintfrancis</t>
+  </si>
+  <si>
+    <t>Pinwheelstreet</t>
+  </si>
+  <si>
+    <t>Antonyrt</t>
+  </si>
+  <si>
+    <t>DateOfBirth</t>
+  </si>
+  <si>
+    <t>2024-07-26T18:14:08.570Z</t>
+  </si>
+  <si>
+    <t>Markty</t>
+  </si>
+  <si>
+    <t>shr10@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -432,8 +476,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62A42F3D-E348-4D43-8D41-01127598F126}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -463,4 +507,96 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{749F9484-35A9-4834-A085-E258A8EE6DD3}">
+  <dimension ref="A1:J2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.44140625" customWidth="1"/>
+    <col min="3" max="3" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>8807306309</v>
+      </c>
+      <c r="B2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2">
+        <v>160741</v>
+      </c>
+      <c r="I2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{148ED1DC-35F8-480A-83E1-399CAC31362C}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Dietitian POST Positive & Negative Tcs
</commit_message>
<xml_diff>
--- a/src/test/resources/Team01_APINinja_Data.xlsx
+++ b/src/test/resources/Team01_APINinja_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Team 1_RestAssured_Shreya\Team01_APINinja_RestAssured\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{671F2152-892C-40F2-8C65-867E25E10276}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B97DF7B4-A580-4365-9865-B3827848A1EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{A03F8C01-D493-49E0-BA62-9B2727C7C8D7}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="33">
   <si>
     <t>password</t>
   </si>
@@ -91,7 +91,40 @@
     <t>Markty</t>
   </si>
   <si>
-    <t>shr10@gmail.com</t>
+    <t>$5</t>
+  </si>
+  <si>
+    <t>$#</t>
+  </si>
+  <si>
+    <t>abc</t>
+  </si>
+  <si>
+    <t>20-07-26T18:14:08.570Z</t>
+  </si>
+  <si>
+    <t>**D</t>
+  </si>
+  <si>
+    <t>%$</t>
+  </si>
+  <si>
+    <t>shrd2@gmail.com</t>
+  </si>
+  <si>
+    <t>shrd3@gmail.com</t>
+  </si>
+  <si>
+    <t>shrd5@gmail.com</t>
+  </si>
+  <si>
+    <t>shrd6@gmail.com</t>
+  </si>
+  <si>
+    <t>shrd10@gmail.com</t>
+  </si>
+  <si>
+    <t>shrd11@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -115,12 +148,30 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -136,9 +187,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -477,7 +532,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+      <selection activeCell="P5" sqref="P5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -511,18 +566,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{749F9484-35A9-4834-A085-E258A8EE6DD3}">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="16.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.44140625" customWidth="1"/>
+    <col min="2" max="2" width="23.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.77734375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.5546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.33203125" bestFit="1" customWidth="1"/>
@@ -563,7 +618,7 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>8807306309</v>
+        <v>5000000300</v>
       </c>
       <c r="B2" t="s">
         <v>19</v>
@@ -572,7 +627,7 @@
         <v>13</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="E2" t="s">
         <v>20</v>
@@ -590,12 +645,279 @@
         <v>16</v>
       </c>
       <c r="J2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" s="2">
+        <v>897676</v>
+      </c>
+      <c r="I3" s="2">
+        <v>89</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H4" s="2">
+        <v>897676</v>
+      </c>
+      <c r="I4" s="2">
+        <v>89</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="2">
+        <v>456</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H5" s="2">
+        <v>897676</v>
+      </c>
+      <c r="I5" s="2">
+        <v>89</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5000000302</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H6" s="2">
+        <v>160741</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>5000000303</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>5000000304</v>
+      </c>
+      <c r="B8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F8" t="s">
+        <v>14</v>
+      </c>
+      <c r="G8" t="s">
+        <v>15</v>
+      </c>
+      <c r="H8">
+        <v>160741</v>
+      </c>
+      <c r="I8" t="s">
+        <v>16</v>
+      </c>
+      <c r="J8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>5000000305</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H9" s="4">
+        <v>160741</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J9" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>5000000306</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H10" s="3">
+        <v>160741</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>5000000307</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H11" s="3">
+        <v>160741</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J11" s="3" t="s">
         <v>17</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" xr:uid="{148ED1DC-35F8-480A-83E1-399CAC31362C}"/>
+    <hyperlink ref="D3:D8" r:id="rId2" display="shrd2@gmail.com" xr:uid="{35F4A9EF-8E5F-410C-A472-E261E6366980}"/>
+    <hyperlink ref="D8" r:id="rId3" xr:uid="{22EF35AB-2F46-4E4F-BA32-0BD94F05ED75}"/>
+    <hyperlink ref="D9" r:id="rId4" xr:uid="{0D38EC72-118F-4EE0-BA2E-856DE2C43369}"/>
+    <hyperlink ref="D10:D11" r:id="rId5" display="shrd4@gmail.com" xr:uid="{EE5DFCDA-4209-48E7-83FD-5F54A83010F5}"/>
+    <hyperlink ref="D10" r:id="rId6" xr:uid="{B9570E8A-C132-44AB-865C-AFE30F8D12D3}"/>
+    <hyperlink ref="D11" r:id="rId7" xr:uid="{0BCB321A-1BF3-4C16-BE77-B129DBAB0891}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Post and put request
</commit_message>
<xml_diff>
--- a/src/test/resources/Team01_APINinja_Data.xlsx
+++ b/src/test/resources/Team01_APINinja_Data.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shanj\vino-workspace\Team01_API_Ninja\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A451BA87-9D74-498B-B57D-CAEA463DC19E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D37188DF-46D6-4B6C-AD93-D013563078EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{A03F8C01-D493-49E0-BA62-9B2727C7C8D7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{A03F8C01-D493-49E0-BA62-9B2727C7C8D7}"/>
   </bookViews>
   <sheets>
     <sheet name="AdminLogin" sheetId="1" r:id="rId1"/>
     <sheet name="PatientPost" sheetId="2" r:id="rId2"/>
+    <sheet name="PatientPut" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="31">
   <si>
     <t>password</t>
   </si>
@@ -90,18 +91,58 @@
     <t>Sam</t>
   </si>
   <si>
-    <t>KAy126@gmail.com</t>
+    <t>Maria</t>
+  </si>
+  <si>
+    <t>Teamone</t>
+  </si>
+  <si>
+    <t>WALNUT</t>
+  </si>
+  <si>
+    <t>Rajasthani</t>
+  </si>
+  <si>
+    <t>KAy131@gmail.com</t>
+  </si>
+  <si>
+    <t>EGGETARIAN</t>
+  </si>
+  <si>
+    <t>Teamoneput</t>
+  </si>
+  <si>
+    <t>Updating only pdf file ,no need to change the data</t>
+  </si>
+  <si>
+    <t>Change any data with pdf file</t>
+  </si>
+  <si>
+    <t>Change any data without pdf</t>
+  </si>
+  <si>
+    <t>update any data with existing pdf file</t>
+  </si>
+  <si>
+    <t>update any date without adding pdf file</t>
+  </si>
+  <si>
+    <t>KAy1350@gmail.com</t>
+  </si>
+  <si>
+    <t>Mario1051@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
     <numFmt numFmtId="165" formatCode="yyyy\-mmdd"/>
+    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -122,6 +163,12 @@
       <color rgb="FF000000"/>
       <name val="Consolas"/>
       <family val="3"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -145,13 +192,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -524,7 +574,120 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2761C07-8EEF-424C-8E2D-5544ABDA6E0C}">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:K3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:H3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.5703125" style="5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="3">
+        <v>3248649250</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" s="2">
+        <v>32110</v>
+      </c>
+      <c r="K2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3">
+        <v>8608306851</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" s="5">
+        <v>31865</v>
+      </c>
+      <c r="K3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{25FC5110-ABF1-4FD8-A244-EDF356B3C1F3}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{61927ED1-99FE-47ED-A36A-F34207D1883B}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C93535F0-6035-4EDE-887A-CE1201C26BCB}">
+  <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H2" sqref="H2"/>
@@ -532,16 +695,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.5703125" style="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -563,22 +725,22 @@
       <c r="G1" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="7" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="C2" s="3">
-        <v>3248649206</v>
+        <v>3248649253</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>13</v>
@@ -589,14 +751,78 @@
       <c r="G2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="H2" s="2">
-        <v>44550</v>
+      <c r="H2" s="8">
+        <v>33967</v>
+      </c>
+      <c r="L2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3">
+        <v>8608306852</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" s="5">
+        <v>31865</v>
+      </c>
+      <c r="L3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4">
+        <v>8608306851</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="H4" s="5">
+        <v>31865</v>
+      </c>
+      <c r="L4" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{25FC5110-ABF1-4FD8-A244-EDF356B3C1F3}"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{5FC30086-0FD1-44DF-94A5-9E22212D0869}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{DB932A1C-5CAF-47A9-8E90-D8C7A057B0E5}"/>
+    <hyperlink ref="D4" r:id="rId3" xr:uid="{EBCDC3F5-7C4B-43D7-B5DA-E56EE05384BE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Dietitian POST & GET completed (Positive & Negative)
</commit_message>
<xml_diff>
--- a/src/test/resources/Team01_APINinja_Data.xlsx
+++ b/src/test/resources/Team01_APINinja_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Team 1_RestAssured_Shreya\Team01_APINinja_RestAssured\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B97DF7B4-A580-4365-9865-B3827848A1EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82B60594-8F0C-41CA-9037-AE931EAF2224}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{A03F8C01-D493-49E0-BA62-9B2727C7C8D7}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="42">
   <si>
     <t>password</t>
   </si>
@@ -121,10 +121,37 @@
     <t>shrd6@gmail.com</t>
   </si>
   <si>
-    <t>shrd10@gmail.com</t>
-  </si>
-  <si>
     <t>shrd11@gmail.com</t>
+  </si>
+  <si>
+    <t>JoJo</t>
+  </si>
+  <si>
+    <t>Jhon</t>
+  </si>
+  <si>
+    <t>shrd47@gmail.com</t>
+  </si>
+  <si>
+    <t>djshfjh</t>
+  </si>
+  <si>
+    <t>put operation on post request</t>
+  </si>
+  <si>
+    <t>invalid end point</t>
+  </si>
+  <si>
+    <t>invalid content type</t>
+  </si>
+  <si>
+    <t>no auth,using dietitian token, patient token</t>
+  </si>
+  <si>
+    <t>shrd70@gmail.com</t>
+  </si>
+  <si>
+    <t>shrd71@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -148,7 +175,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -157,19 +184,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -190,10 +205,10 @@
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -566,10 +581,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{749F9484-35A9-4834-A085-E258A8EE6DD3}">
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -582,9 +597,10 @@
     <col min="7" max="7" width="12.5546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="24.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -616,50 +632,53 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>5000000300</v>
-      </c>
-      <c r="B2" t="s">
+    <row r="2" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2">
+        <v>5000001000</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="D2" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="2">
         <v>160741</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="2">
+        <v>5000001001</v>
+      </c>
       <c r="B3" s="2" t="s">
         <v>19</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>27</v>
+        <v>13</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>14</v>
@@ -668,26 +687,24 @@
         <v>15</v>
       </c>
       <c r="H3" s="2">
-        <v>897676</v>
-      </c>
-      <c r="I3" s="2">
-        <v>89</v>
+        <v>160741</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>22</v>
-      </c>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="4"/>
       <c r="B4" s="2" t="s">
         <v>19</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="3" t="s">
         <v>27</v>
       </c>
       <c r="E4" s="2" t="s">
@@ -709,9 +726,9 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="2">
-        <v>456</v>
+    <row r="5" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
+        <v>22</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>19</v>
@@ -719,7 +736,7 @@
       <c r="C5" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="3" t="s">
         <v>27</v>
       </c>
       <c r="E5" s="2" t="s">
@@ -741,14 +758,17 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>5000000302</v>
+    <row r="6" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="4">
+        <v>456</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>27</v>
       </c>
       <c r="E6" s="2" t="s">
@@ -761,163 +781,242 @@
         <v>15</v>
       </c>
       <c r="H6" s="2">
+        <v>897676</v>
+      </c>
+      <c r="I6" s="2">
+        <v>89</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="2">
+        <v>5000001002</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H7" s="4">
+        <v>53</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="2">
+        <v>5000001003</v>
+      </c>
+      <c r="B8" s="4"/>
+      <c r="C8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="3"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
+    </row>
+    <row r="9" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="2">
+        <v>5000001004</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H9" s="2">
         <v>160741</v>
       </c>
-      <c r="I6" s="2" t="s">
+      <c r="I9" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="J6" s="2" t="s">
+      <c r="J9" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="2">
+        <v>5000001005</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H10" s="2">
+        <v>160741</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J10" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>5000000303</v>
-      </c>
-      <c r="C7" s="2" t="s">
+      <c r="K10" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="2">
+        <v>5000001006</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>5000000304</v>
-      </c>
-      <c r="B8" t="s">
+      <c r="D11" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H11" s="2">
+        <v>160741</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="2">
+        <v>5000001007</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C12" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E8" t="s">
-        <v>25</v>
-      </c>
-      <c r="F8" t="s">
+      <c r="D12" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F12" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G8" t="s">
+      <c r="G12" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="H8">
+      <c r="H12" s="2">
         <v>160741</v>
       </c>
-      <c r="I8" t="s">
+      <c r="I12" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="J8" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <v>5000000305</v>
-      </c>
-      <c r="B9" s="4" t="s">
+      <c r="J12" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="2">
+        <v>5000001008</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C13" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="F9" s="4" t="s">
+      <c r="D13" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F13" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G9" s="4" t="s">
+      <c r="G13" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="H9" s="4">
+      <c r="H13" s="2">
         <v>160741</v>
       </c>
-      <c r="I9" s="4" t="s">
+      <c r="I13" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="J9" s="4" t="s">
+      <c r="J13" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A10">
-        <v>5000000306</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="H10" s="3">
-        <v>160741</v>
-      </c>
-      <c r="I10" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="J10" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A11">
-        <v>5000000307</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="H11" s="3">
-        <v>160741</v>
-      </c>
-      <c r="I11" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="J11" s="3" t="s">
-        <v>17</v>
+      <c r="K13" s="2" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" xr:uid="{148ED1DC-35F8-480A-83E1-399CAC31362C}"/>
-    <hyperlink ref="D3:D8" r:id="rId2" display="shrd2@gmail.com" xr:uid="{35F4A9EF-8E5F-410C-A472-E261E6366980}"/>
-    <hyperlink ref="D8" r:id="rId3" xr:uid="{22EF35AB-2F46-4E4F-BA32-0BD94F05ED75}"/>
-    <hyperlink ref="D9" r:id="rId4" xr:uid="{0D38EC72-118F-4EE0-BA2E-856DE2C43369}"/>
-    <hyperlink ref="D10:D11" r:id="rId5" display="shrd4@gmail.com" xr:uid="{EE5DFCDA-4209-48E7-83FD-5F54A83010F5}"/>
-    <hyperlink ref="D10" r:id="rId6" xr:uid="{B9570E8A-C132-44AB-865C-AFE30F8D12D3}"/>
-    <hyperlink ref="D11" r:id="rId7" xr:uid="{0BCB321A-1BF3-4C16-BE77-B129DBAB0891}"/>
+    <hyperlink ref="D9" r:id="rId2" xr:uid="{22EF35AB-2F46-4E4F-BA32-0BD94F05ED75}"/>
+    <hyperlink ref="D10" r:id="rId3" xr:uid="{0D38EC72-118F-4EE0-BA2E-856DE2C43369}"/>
+    <hyperlink ref="D11:D12" r:id="rId4" display="shrd4@gmail.com" xr:uid="{EE5DFCDA-4209-48E7-83FD-5F54A83010F5}"/>
+    <hyperlink ref="D11" r:id="rId5" xr:uid="{B9570E8A-C132-44AB-865C-AFE30F8D12D3}"/>
+    <hyperlink ref="D12" r:id="rId6" xr:uid="{0BCB321A-1BF3-4C16-BE77-B129DBAB0891}"/>
+    <hyperlink ref="D13" r:id="rId7" xr:uid="{7F020AD9-0287-441A-A836-7EAA8314E224}"/>
+    <hyperlink ref="D3" r:id="rId8" xr:uid="{4FE9774A-4B22-460C-81E1-E1B57FC82D7A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
POST and PUT Negative
</commit_message>
<xml_diff>
--- a/src/test/resources/Team01_APINinja_Data.xlsx
+++ b/src/test/resources/Team01_APINinja_Data.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shanj\vino-workspace\Team01_API_Ninja\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D37188DF-46D6-4B6C-AD93-D013563078EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDBDE69F-6F56-47B0-A80B-6A69B9037C0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{A03F8C01-D493-49E0-BA62-9B2727C7C8D7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A03F8C01-D493-49E0-BA62-9B2727C7C8D7}"/>
   </bookViews>
   <sheets>
     <sheet name="AdminLogin" sheetId="1" r:id="rId1"/>
     <sheet name="PatientPost" sheetId="2" r:id="rId2"/>
     <sheet name="PatientPut" sheetId="3" r:id="rId3"/>
+    <sheet name="Patientputvital" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="52">
   <si>
     <t>password</t>
   </si>
@@ -112,25 +113,88 @@
     <t>Teamoneput</t>
   </si>
   <si>
-    <t>Updating only pdf file ,no need to change the data</t>
-  </si>
-  <si>
     <t>Change any data with pdf file</t>
   </si>
   <si>
     <t>Change any data without pdf</t>
   </si>
   <si>
-    <t>update any data with existing pdf file</t>
-  </si>
-  <si>
-    <t>update any date without adding pdf file</t>
-  </si>
-  <si>
     <t>KAy1350@gmail.com</t>
   </si>
   <si>
     <t>Mario1051@gmail.com</t>
+  </si>
+  <si>
+    <t>invalid Mandatory data</t>
+  </si>
+  <si>
+    <t>Sue12</t>
+  </si>
+  <si>
+    <t>katie1</t>
+  </si>
+  <si>
+    <t>jaf54@gmail.com</t>
+  </si>
+  <si>
+    <t>123-12-30</t>
+  </si>
+  <si>
+    <t>Ram</t>
+  </si>
+  <si>
+    <t>Swamy</t>
+  </si>
+  <si>
+    <t>Ramy@gmail.com</t>
+  </si>
+  <si>
+    <t>Valid Mandatory invalid additional field</t>
+  </si>
+  <si>
+    <t>Ve%gan</t>
+  </si>
+  <si>
+    <t>Tamil</t>
+  </si>
+  <si>
+    <t>Vega</t>
+  </si>
+  <si>
+    <t xml:space="preserve">update any data focus only Mandatory and additional details  without adding pdf file  (update either email or DOB) </t>
+  </si>
+  <si>
+    <t>Updating only pdf file ,no need to change the data(NO data update)</t>
+  </si>
+  <si>
+    <t>update any data with existing pdf file (update either contact number or food preference)</t>
+  </si>
+  <si>
+    <t>Positive</t>
+  </si>
+  <si>
+    <t>Negative</t>
+  </si>
+  <si>
+    <t>invalid additional field</t>
+  </si>
+  <si>
+    <t>Wal@nut</t>
+  </si>
+  <si>
+    <t>West Vegan</t>
+  </si>
+  <si>
+    <t>Indiaaa</t>
+  </si>
+  <si>
+    <t>team123@gmail.com</t>
+  </si>
+  <si>
+    <t>Valid data</t>
+  </si>
+  <si>
+    <t>invalid data</t>
   </si>
 </sst>
 </file>
@@ -537,10 +601,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62A42F3D-E348-4D43-8D41-01127598F126}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -548,7 +612,7 @@
     <col min="2" max="2" width="17.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -556,17 +620,32 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>3</v>
+      </c>
+      <c r="E2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E3" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{4EBEBFA7-2488-42FB-B465-9C193BD3C70E}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{C52AFF14-183F-404A-A159-9C5E46F6B1F0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -574,10 +653,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2761C07-8EEF-424C-8E2D-5544ABDA6E0C}">
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:H3"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -588,7 +667,7 @@
     <col min="4" max="4" width="20.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.5703125" style="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
@@ -613,7 +692,7 @@
       <c r="G1" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="7" t="s">
         <v>11</v>
       </c>
     </row>
@@ -628,7 +707,7 @@
         <v>3248649250</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>13</v>
@@ -639,11 +718,11 @@
       <c r="G2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="H2" s="2">
+      <c r="H2" s="8">
         <v>32110</v>
       </c>
       <c r="K2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="17.25" x14ac:dyDescent="0.3">
@@ -657,7 +736,7 @@
         <v>8608306851</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E3" t="s">
         <v>19</v>
@@ -668,29 +747,89 @@
       <c r="G3" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="H3" s="5">
+      <c r="H3" s="7">
         <v>31865</v>
       </c>
       <c r="K3" t="s">
-        <v>26</v>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6">
+        <v>3457899</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" t="s">
+        <v>37</v>
+      </c>
+      <c r="G6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="K6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7">
+        <v>8408305647</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" t="s">
+        <v>39</v>
+      </c>
+      <c r="G7" t="s">
+        <v>38</v>
+      </c>
+      <c r="H7" s="7">
+        <v>31865</v>
+      </c>
+      <c r="K7" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" xr:uid="{25FC5110-ABF1-4FD8-A244-EDF356B3C1F3}"/>
     <hyperlink ref="D3" r:id="rId2" xr:uid="{61927ED1-99FE-47ED-A36A-F34207D1883B}"/>
+    <hyperlink ref="D6" r:id="rId3" xr:uid="{3AC634B2-EE07-47BC-8F0A-8DE85105F4CD}"/>
+    <hyperlink ref="D7" r:id="rId4" xr:uid="{4C4FBBF4-4DBC-4035-B8E5-3DCFE6E11CBB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C93535F0-6035-4EDE-887A-CE1201C26BCB}">
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:L6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -754,75 +893,157 @@
       <c r="H2" s="8">
         <v>33967</v>
       </c>
+      <c r="K2" t="s">
+        <v>43</v>
+      </c>
       <c r="L2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3">
-        <v>8608306852</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="H3" s="5">
-        <v>31865</v>
+        <v>23</v>
+      </c>
+      <c r="C3" s="3">
+        <v>3248649253</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" s="8">
+        <v>33967</v>
+      </c>
+      <c r="K3" t="s">
+        <v>43</v>
       </c>
       <c r="L3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4">
-        <v>8608306851</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="H4" s="5">
-        <v>31865</v>
+        <v>23</v>
+      </c>
+      <c r="C4" s="3">
+        <v>3248649253</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H4" s="8">
+        <v>33967</v>
+      </c>
+      <c r="K4" t="s">
+        <v>43</v>
       </c>
       <c r="L4" t="s">
-        <v>24</v>
-      </c>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="3">
+        <v>3248649253</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="H5" s="8">
+        <v>33967</v>
+      </c>
+      <c r="K5" t="s">
+        <v>44</v>
+      </c>
+      <c r="L5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C6" s="3"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="8"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" xr:uid="{5FC30086-0FD1-44DF-94A5-9E22212D0869}"/>
-    <hyperlink ref="D3" r:id="rId2" xr:uid="{DB932A1C-5CAF-47A9-8E90-D8C7A057B0E5}"/>
-    <hyperlink ref="D4" r:id="rId3" xr:uid="{EBCDC3F5-7C4B-43D7-B5DA-E56EE05384BE}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{A2D994B3-51BC-42B8-AF2E-6454766E2303}"/>
+    <hyperlink ref="D4" r:id="rId3" xr:uid="{3987B665-0136-4C24-9EFD-057587B1C236}"/>
+    <hyperlink ref="D5" r:id="rId4" xr:uid="{0F3A3A78-92A9-48FC-9C8A-FB9AF8FD3B22}"/>
+    <hyperlink ref="E5" r:id="rId5" xr:uid="{7650373E-8BAB-4A22-B95F-F0627991A046}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId4"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId6"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1507267-6321-4AFA-A423-A62ECE9DF42B}">
+  <dimension ref="D1:H2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="H1" s="7"/>
+    </row>
+    <row r="2" spans="4:8" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="D2" s="1"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="5"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Dietitian PUT & Delete Updated positive flow
</commit_message>
<xml_diff>
--- a/src/test/resources/Team01_APINinja_Data.xlsx
+++ b/src/test/resources/Team01_APINinja_Data.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Team 1_RestAssured_Shreya\Team01_APINinja_RestAssured\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82B60594-8F0C-41CA-9037-AE931EAF2224}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEEB7EA9-B585-405D-9EBF-BF1015F7A639}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{A03F8C01-D493-49E0-BA62-9B2727C7C8D7}"/>
   </bookViews>
   <sheets>
     <sheet name="AdminLogin" sheetId="1" r:id="rId1"/>
     <sheet name="DietitianPost" sheetId="2" r:id="rId2"/>
+    <sheet name="DietitianPut" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="50">
   <si>
     <t>password</t>
   </si>
@@ -148,10 +149,34 @@
     <t>no auth,using dietitian token, patient token</t>
   </si>
   <si>
-    <t>shrd70@gmail.com</t>
-  </si>
-  <si>
-    <t>shrd71@gmail.com</t>
+    <t>JhonM</t>
+  </si>
+  <si>
+    <t>HartfordC</t>
+  </si>
+  <si>
+    <t>SaintfrancisC</t>
+  </si>
+  <si>
+    <t>kk</t>
+  </si>
+  <si>
+    <t>MM</t>
+  </si>
+  <si>
+    <t>2024-07-29T18:14:08.570Z</t>
+  </si>
+  <si>
+    <t>shre1@gmail.com</t>
+  </si>
+  <si>
+    <t>BTEch1</t>
+  </si>
+  <si>
+    <t>shrd90@gmail.com</t>
+  </si>
+  <si>
+    <t>shrd91@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -202,10 +227,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1"/>
@@ -547,7 +571,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P5" sqref="P5"/>
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -584,7 +608,7 @@
   <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -632,378 +656,378 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2">
-        <v>5000001000</v>
-      </c>
-      <c r="B2" s="2" t="s">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>5000002014</v>
+      </c>
+      <c r="B2" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="E2" s="2" t="s">
+      <c r="D2" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E2" t="s">
         <v>33</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" t="s">
         <v>15</v>
       </c>
-      <c r="H2" s="2">
+      <c r="H2">
         <v>160741</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="I2" t="s">
         <v>16</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="J2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="2">
-        <v>5000001001</v>
-      </c>
-      <c r="B3" s="2" t="s">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>5000002015</v>
+      </c>
+      <c r="B3" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="E3" s="2" t="s">
+      <c r="D3" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E3" t="s">
         <v>32</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G3" t="s">
         <v>15</v>
       </c>
-      <c r="H3" s="2">
+      <c r="H3">
         <v>160741</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="I3" t="s">
         <v>16</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="J3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="4"/>
-      <c r="B4" s="2" t="s">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" s="3"/>
+      <c r="B4" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" t="s">
         <v>20</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F4" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="G4" t="s">
         <v>15</v>
       </c>
-      <c r="H4" s="2">
+      <c r="H4">
         <v>897676</v>
       </c>
-      <c r="I4" s="2">
+      <c r="I4">
         <v>89</v>
       </c>
-      <c r="J4" s="2" t="s">
+      <c r="J4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" t="s">
         <v>20</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="F5" t="s">
         <v>14</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="G5" t="s">
         <v>15</v>
       </c>
-      <c r="H5" s="2">
+      <c r="H5">
         <v>897676</v>
       </c>
-      <c r="I5" s="2">
+      <c r="I5">
         <v>89</v>
       </c>
-      <c r="J5" s="2" t="s">
+      <c r="J5" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="4">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" s="3">
         <v>456</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E6" t="s">
         <v>20</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="F6" t="s">
         <v>14</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="G6" t="s">
         <v>15</v>
       </c>
-      <c r="H6" s="2">
+      <c r="H6">
         <v>897676</v>
       </c>
-      <c r="I6" s="2">
+      <c r="I6">
         <v>89</v>
       </c>
-      <c r="J6" s="2" t="s">
+      <c r="J6" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A7">
         <v>5000001002</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="E7" t="s">
         <v>20</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="F7" t="s">
         <v>14</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="G7" t="s">
         <v>15</v>
       </c>
-      <c r="H7" s="4">
+      <c r="H7" s="3">
         <v>53</v>
       </c>
-      <c r="I7" s="2" t="s">
+      <c r="I7" t="s">
         <v>16</v>
       </c>
-      <c r="J7" s="2" t="s">
+      <c r="J7" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A8">
         <v>5000001003</v>
       </c>
-      <c r="B8" s="4"/>
-      <c r="C8" s="2" t="s">
+      <c r="B8" s="3"/>
+      <c r="C8" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="3"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
-      <c r="J8" s="4"/>
-    </row>
-    <row r="9" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="2">
+      <c r="D8" s="2"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9">
         <v>5000001004</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="E9" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="F9" t="s">
         <v>14</v>
       </c>
-      <c r="G9" s="2" t="s">
+      <c r="G9" t="s">
         <v>15</v>
       </c>
-      <c r="H9" s="2">
+      <c r="H9">
         <v>160741</v>
       </c>
-      <c r="I9" s="2" t="s">
+      <c r="I9" t="s">
         <v>16</v>
       </c>
-      <c r="J9" s="4" t="s">
+      <c r="J9" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10">
         <v>5000001005</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" t="s">
         <v>13</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D10" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="E10" t="s">
         <v>20</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="F10" t="s">
         <v>14</v>
       </c>
-      <c r="G10" s="2" t="s">
+      <c r="G10" t="s">
         <v>15</v>
       </c>
-      <c r="H10" s="2">
+      <c r="H10">
         <v>160741</v>
       </c>
-      <c r="I10" s="2" t="s">
+      <c r="I10" t="s">
         <v>16</v>
       </c>
-      <c r="J10" s="2" t="s">
+      <c r="J10" t="s">
         <v>17</v>
       </c>
-      <c r="K10" s="2" t="s">
+      <c r="K10" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11">
         <v>5000001006</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" t="s">
         <v>13</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D11" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="E11" t="s">
         <v>20</v>
       </c>
-      <c r="F11" s="2" t="s">
+      <c r="F11" t="s">
         <v>14</v>
       </c>
-      <c r="G11" s="2" t="s">
+      <c r="G11" t="s">
         <v>15</v>
       </c>
-      <c r="H11" s="2">
+      <c r="H11">
         <v>160741</v>
       </c>
-      <c r="I11" s="2" t="s">
+      <c r="I11" t="s">
         <v>16</v>
       </c>
-      <c r="J11" s="2" t="s">
+      <c r="J11" t="s">
         <v>17</v>
       </c>
-      <c r="K11" s="2" t="s">
+      <c r="K11" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A12">
         <v>5000001007</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" t="s">
         <v>13</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="D12" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="E12" t="s">
         <v>20</v>
       </c>
-      <c r="F12" s="2" t="s">
+      <c r="F12" t="s">
         <v>14</v>
       </c>
-      <c r="G12" s="2" t="s">
+      <c r="G12" t="s">
         <v>15</v>
       </c>
-      <c r="H12" s="2">
+      <c r="H12">
         <v>160741</v>
       </c>
-      <c r="I12" s="2" t="s">
+      <c r="I12" t="s">
         <v>16</v>
       </c>
-      <c r="J12" s="2" t="s">
+      <c r="J12" t="s">
         <v>17</v>
       </c>
-      <c r="K12" s="2" t="s">
+      <c r="K12" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A13">
         <v>5000001008</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" t="s">
         <v>13</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="D13" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="E13" t="s">
         <v>33</v>
       </c>
-      <c r="F13" s="2" t="s">
+      <c r="F13" t="s">
         <v>14</v>
       </c>
-      <c r="G13" s="2" t="s">
+      <c r="G13" t="s">
         <v>15</v>
       </c>
-      <c r="H13" s="2">
+      <c r="H13">
         <v>160741</v>
       </c>
-      <c r="I13" s="2" t="s">
+      <c r="I13" t="s">
         <v>16</v>
       </c>
-      <c r="J13" s="2" t="s">
+      <c r="J13" t="s">
         <v>17</v>
       </c>
-      <c r="K13" s="2" t="s">
+      <c r="K13" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1020,4 +1044,97 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D50FE735-FDD6-4232-806D-9C0403FC55E2}">
+  <dimension ref="A1:J2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>5000002540</v>
+      </c>
+      <c r="B2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F2" t="s">
+        <v>41</v>
+      </c>
+      <c r="G2" t="s">
+        <v>42</v>
+      </c>
+      <c r="H2">
+        <v>100000</v>
+      </c>
+      <c r="I2" t="s">
+        <v>43</v>
+      </c>
+      <c r="J2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{9E71020C-F5B4-44B9-8596-92A2E9F7A032}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Postive and Negative TC
</commit_message>
<xml_diff>
--- a/src/test/resources/Team01_APINinja_Data.xlsx
+++ b/src/test/resources/Team01_APINinja_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shanj\vino-workspace\Team01_API_Ninja\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDBDE69F-6F56-47B0-A80B-6A69B9037C0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{177F4019-F343-4A87-96C8-36806A709A4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A03F8C01-D493-49E0-BA62-9B2727C7C8D7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{A03F8C01-D493-49E0-BA62-9B2727C7C8D7}"/>
   </bookViews>
   <sheets>
     <sheet name="AdminLogin" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="57">
   <si>
     <t>password</t>
   </si>
@@ -119,12 +119,6 @@
     <t>Change any data without pdf</t>
   </si>
   <si>
-    <t>KAy1350@gmail.com</t>
-  </si>
-  <si>
-    <t>Mario1051@gmail.com</t>
-  </si>
-  <si>
     <t>invalid Mandatory data</t>
   </si>
   <si>
@@ -195,16 +189,36 @@
   </si>
   <si>
     <t>invalid data</t>
+  </si>
+  <si>
+    <t>Weight</t>
+  </si>
+  <si>
+    <t>Height</t>
+  </si>
+  <si>
+    <t>Temperature</t>
+  </si>
+  <si>
+    <t>SP</t>
+  </si>
+  <si>
+    <t>DP</t>
+  </si>
+  <si>
+    <t>KAy1354@gmail.com</t>
+  </si>
+  <si>
+    <t>Mario1065@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
-    <numFmt numFmtId="165" formatCode="yyyy\-mmdd"/>
-    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -256,16 +270,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -603,7 +616,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62A42F3D-E348-4D43-8D41-01127598F126}">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
@@ -628,7 +641,7 @@
         <v>3</v>
       </c>
       <c r="E2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -636,10 +649,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E3" t="s">
         <v>49</v>
-      </c>
-      <c r="E3" t="s">
-        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -655,8 +668,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2761C07-8EEF-424C-8E2D-5544ABDA6E0C}">
   <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -667,7 +680,7 @@
     <col min="4" max="4" width="20.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.5703125" style="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
@@ -692,7 +705,7 @@
       <c r="G1" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="H1" s="6" t="s">
         <v>11</v>
       </c>
     </row>
@@ -704,10 +717,10 @@
         <v>12</v>
       </c>
       <c r="C2" s="3">
-        <v>3248649250</v>
+        <v>3248649254</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>26</v>
+        <v>55</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>13</v>
@@ -718,8 +731,8 @@
       <c r="G2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="H2" s="8">
-        <v>32110</v>
+      <c r="H2" s="7">
+        <v>32476</v>
       </c>
       <c r="K2" t="s">
         <v>24</v>
@@ -733,10 +746,10 @@
         <v>18</v>
       </c>
       <c r="C3">
-        <v>8608306851</v>
+        <v>8608306865</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>27</v>
+        <v>56</v>
       </c>
       <c r="E3" t="s">
         <v>19</v>
@@ -744,11 +757,11 @@
       <c r="F3" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="H3" s="7">
-        <v>31865</v>
+      <c r="H3" s="6">
+        <v>32227</v>
       </c>
       <c r="K3" t="s">
         <v>25</v>
@@ -756,60 +769,60 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C6">
         <v>3457899</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E6" t="s">
         <v>13</v>
       </c>
       <c r="F6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G6" t="s">
         <v>15</v>
       </c>
-      <c r="H6" s="7" t="s">
-        <v>32</v>
+      <c r="H6" s="6" t="s">
+        <v>30</v>
       </c>
       <c r="K6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C7">
         <v>8408305647</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E7" t="s">
         <v>13</v>
       </c>
       <c r="F7" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G7" t="s">
-        <v>38</v>
-      </c>
-      <c r="H7" s="7">
+        <v>36</v>
+      </c>
+      <c r="H7" s="6">
         <v>31865</v>
       </c>
       <c r="K7" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -839,7 +852,7 @@
     <col min="3" max="3" width="21.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.5703125" style="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -864,7 +877,7 @@
       <c r="G1" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="H1" s="6" t="s">
         <v>11</v>
       </c>
     </row>
@@ -890,14 +903,14 @@
       <c r="G2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="H2" s="8">
+      <c r="H2" s="7">
         <v>33967</v>
       </c>
       <c r="K2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="L2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -922,14 +935,14 @@
       <c r="G3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="H3" s="8">
+      <c r="H3" s="7">
         <v>33967</v>
       </c>
       <c r="K3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="L3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -954,14 +967,14 @@
       <c r="G4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="H4" s="8">
+      <c r="H4" s="7">
         <v>33967</v>
       </c>
       <c r="K4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="L4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -978,22 +991,22 @@
         <v>21</v>
       </c>
       <c r="E5" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G5" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="F5" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="H5" s="8">
+      <c r="H5" s="7">
         <v>33967</v>
       </c>
       <c r="K5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="L5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -1002,7 +1015,7 @@
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
-      <c r="H6" s="8"/>
+      <c r="H6" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1019,29 +1032,47 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1507267-6321-4AFA-A423-A62ECE9DF42B}">
-  <dimension ref="D1:H2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="3" max="3" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.5703125" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="H1" s="7"/>
-    </row>
-    <row r="2" spans="4:8" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="D2" s="1"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="5"/>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>70.2</v>
+      </c>
+      <c r="B2">
+        <v>165.5</v>
+      </c>
+      <c r="C2">
+        <v>98.3</v>
+      </c>
+      <c r="D2">
+        <v>34</v>
+      </c>
+      <c r="E2">
+        <v>56</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>